<commit_message>
onInterpolation 함수 & forceChangeResolution
</commit_message>
<xml_diff>
--- a/datas/db.xlsx
+++ b/datas/db.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dano Sato\Documents\Python\REMO-Engine-100Examples\datas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8952B4EF-3EC1-4BDA-B8E7-54D92DD02487}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C061761F-A2AE-4CEF-A597-6CF872044402}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8240" yWindow="4450" windowWidth="28800" windowHeight="15380" activeTab="2" xr2:uid="{E60D345E-077A-4973-BE7F-27EB13B8077E}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" activeTab="2" xr2:uid="{E60D345E-077A-4973-BE7F-27EB13B8077E}"/>
   </bookViews>
   <sheets>
     <sheet name="item" sheetId="1" r:id="rId1"/>
@@ -188,11 +188,11 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>long long text example to check my library is ok.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>매우 긴 문장을 한번 써봐서 이것도 잘 되는지 볼려구 해요.</t>
+    <t>A를 눌러서 한국어로 바꾸고, S키눌러서 영어로 바꿔보세요.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Press A to make Korean, press S to make English</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -780,7 +780,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -828,10 +828,10 @@
         <v>40</v>
       </c>
       <c r="B4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C4" t="s">
         <v>41</v>
-      </c>
-      <c r="C4" t="s">
-        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>